<commit_message>
update 5a_prototype, this closes #3
</commit_message>
<xml_diff>
--- a/planning/5a_prototype.xlsx
+++ b/planning/5a_prototype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EthienneC/Desktop/5a/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C89686F-5BED-0842-B802-9DE680F15303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D35ED3B-1936-CF4A-8FB5-E82E012AF742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="1 entre x" sheetId="5" r:id="rId3"/>
     <sheet name="t-student" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2358,7 +2358,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2401,7 +2401,7 @@
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f>(C2-C1)/C3</f>
         <v>0.25</v>
       </c>

</xml_diff>